<commit_message>
Thêm Q&A,sửa 1 lỗi chính tả trong Requirments
</commit_message>
<xml_diff>
--- a/Document/1_Req/Q&A.xlsx
+++ b/Document/1_Req/Q&A.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
   <si>
     <t>No</t>
   </si>
@@ -128,6 +128,49 @@
   </si>
   <si>
     <t>TuNT</t>
+  </si>
+  <si>
+    <t>Có phải là số lượng cảnh báo chỉ giảm khi bấm vào 1 Item trong Danh sách công việc/công văn không?</t>
+  </si>
+  <si>
+    <t>ToanNM</t>
+  </si>
+  <si>
+    <t>Sau khi thêm công việc mới thì công việc mới
+đó sẽ  ở trong Mục nào(Tất cả cv,cv được giao,
+công việc đã giao,công việc theo dõi hay cv 
+đã hoàn thành)?</t>
+  </si>
+  <si>
+    <t>Tìm kiếm công việc sẽ tìm theo 1 danh sách có 
+sẵn(autoComplete)hay phải nhập đầy đủ tên
+Công việc hoặc tên người giao/được giao?</t>
+  </si>
+  <si>
+    <t>Trong màn hình lọc công việc theo phòng ban,
+khi có 1 công việc được giao cho 2 hoặc nhiều
+phòng ban thì sẽ hiển thị tên công việc ở cả 2 
+màn hình đúng không?</t>
+  </si>
+  <si>
+    <t>Màn hình Chi tiết CV cho phép sửa chi tiết CV
+vậy User có quyền sửa những thông tin nào về
+CV?</t>
+  </si>
+  <si>
+    <t>Màn hình Thêm CV,phòng ban được tự động
+và không cho người dùng nhập liệu.Vậy khi tạo
+mới 1 CV,mặc định sẽ là phòng ban nào nhận
+CV đó?</t>
+  </si>
+  <si>
+    <t>Trong màn hình Tìm kiếm,khi người dùng chọn
+CV được giao/đã giao và nhập tên CV/người 
+thì sẽ tìm trong CV được giao/đã giao hay tìm theo Tất cả CV hiện có?</t>
+  </si>
+  <si>
+    <t>Danh sách Công văn hiển thị ngắn gọn Công văn 
+Đúng không?</t>
   </si>
 </sst>
 </file>
@@ -138,7 +181,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -517,33 +560,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.75" customWidth="1"/>
-    <col min="3" max="3" width="39.875" customWidth="1"/>
-    <col min="4" max="4" width="14.25" customWidth="1"/>
-    <col min="5" max="5" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" customWidth="1"/>
+    <col min="3" max="3" width="39.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2">
         <f>COUNTIF(G8:G41,G2)</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -555,7 +598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -567,16 +610,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5">
         <f>SUM(C2:C4)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,7 +642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -616,7 +659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -633,7 +676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -650,7 +693,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>4</v>
       </c>
@@ -669,7 +712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="57" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>5</v>
       </c>
@@ -688,7 +731,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="57" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>6</v>
       </c>
@@ -707,7 +750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>7</v>
       </c>
@@ -726,7 +769,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>8</v>
       </c>
@@ -745,7 +788,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9</v>
       </c>
@@ -764,7 +807,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
@@ -783,7 +826,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
@@ -802,7 +845,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="57" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>
@@ -821,7 +864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>13</v>
       </c>
@@ -840,102 +883,198 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="3">
+        <v>41921</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="3">
+        <v>41921</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="3">
+        <v>41921</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="3">
+        <v>41921</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="3">
+        <v>41921</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="3">
+        <v>41921</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="3">
+        <v>41921</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="3">
+        <v>41921</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>33</v>
       </c>
@@ -956,7 +1095,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -968,7 +1107,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>